<commit_message>
Snapshot    20180103-1 Add:        1. Clean pipline for K-fold validation             2. Compile result into Excel Note:       1. Input channel: 2    (QSM, R2S)             2. Extraction step: 3x3x3             3. No Fine-tune step             4. K = 10
</commit_message>
<xml_diff>
--- a/results/compile.xlsx
+++ b/results/compile.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="K10_QSM_R2S" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="K10_QSM_R2S_noFT" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="25">
   <si>
     <t xml:space="preserve">Precision</t>
   </si>
@@ -220,12 +221,12 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I32" activeCellId="0" sqref="I32"/>
+      <selection pane="topLeft" activeCell="E36" activeCellId="0" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -233,6 +234,18 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
+      <c r="M1" s="0"/>
+      <c r="N1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -401,7 +414,7 @@
       </c>
       <c r="N5" s="4" t="n">
         <f aca="false">STDEV(B5:K5)</f>
-        <v>0.0563789029198373</v>
+        <v>0.0563789029198374</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -705,12 +718,52 @@
         <v>0.0976809717908253</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0"/>
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
+      <c r="D13" s="0"/>
+      <c r="E13" s="0"/>
+      <c r="F13" s="0"/>
+      <c r="G13" s="0"/>
+      <c r="H13" s="0"/>
+      <c r="I13" s="0"/>
+      <c r="J13" s="0"/>
+      <c r="K13" s="0"/>
+      <c r="M13" s="0"/>
+      <c r="N13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="0"/>
+      <c r="C14" s="0"/>
+      <c r="D14" s="0"/>
+      <c r="E14" s="0"/>
+      <c r="F14" s="0"/>
+      <c r="G14" s="0"/>
+      <c r="H14" s="0"/>
+      <c r="I14" s="0"/>
+      <c r="J14" s="0"/>
+      <c r="K14" s="0"/>
+      <c r="M14" s="0"/>
+      <c r="N14" s="0"/>
+    </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="B15" s="0"/>
+      <c r="C15" s="0"/>
+      <c r="D15" s="0"/>
+      <c r="E15" s="0"/>
+      <c r="F15" s="0"/>
+      <c r="G15" s="0"/>
+      <c r="H15" s="0"/>
+      <c r="I15" s="0"/>
+      <c r="J15" s="0"/>
+      <c r="K15" s="0"/>
+      <c r="M15" s="0"/>
+      <c r="N15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
@@ -1192,4 +1245,984 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:N26"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L30" activeCellId="0" sqref="L30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="n">
+        <v>0.9155</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>0.86075</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>0.9453</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>0.9277</v>
+      </c>
+      <c r="G3" s="4" t="n">
+        <v>0.4634</v>
+      </c>
+      <c r="H3" s="4" t="n">
+        <v>0.9364</v>
+      </c>
+      <c r="I3" s="4" t="n">
+        <v>0.4817</v>
+      </c>
+      <c r="J3" s="4" t="n">
+        <v>0.90915</v>
+      </c>
+      <c r="K3" s="4" t="n">
+        <v>0.97335</v>
+      </c>
+      <c r="M3" s="4" t="n">
+        <f aca="false">AVERAGE(B3:K3)</f>
+        <v>0.778825</v>
+      </c>
+      <c r="N3" s="4" t="n">
+        <f aca="false">STDEV(B3:K3)</f>
+        <v>0.237059472437239</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4" t="n">
+        <v>0.8654</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>0.4077</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>0.96925</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>0.87675</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>0.85375</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>0.81355</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>0.9298</v>
+      </c>
+      <c r="I4" s="4" t="n">
+        <v>0.93765</v>
+      </c>
+      <c r="J4" s="4" t="n">
+        <v>0.90625</v>
+      </c>
+      <c r="K4" s="4" t="n">
+        <v>0.8574</v>
+      </c>
+      <c r="M4" s="4" t="n">
+        <f aca="false">AVERAGE(B4:K4)</f>
+        <v>0.84175</v>
+      </c>
+      <c r="N4" s="4" t="n">
+        <f aca="false">STDEV(B4:K4)</f>
+        <v>0.159420478260758</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>0.92685</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>0.88215</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>0.49165</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>0.4453</v>
+      </c>
+      <c r="F5" s="4" t="n">
+        <v>0.35745</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>0.83095</v>
+      </c>
+      <c r="H5" s="4" t="n">
+        <v>0.9652</v>
+      </c>
+      <c r="I5" s="4" t="n">
+        <v>0.85285</v>
+      </c>
+      <c r="J5" s="4" t="n">
+        <v>0.90945</v>
+      </c>
+      <c r="K5" s="4" t="n">
+        <v>0.9316</v>
+      </c>
+      <c r="M5" s="4" t="n">
+        <f aca="false">AVERAGE(B5:K5)</f>
+        <v>0.759345</v>
+      </c>
+      <c r="N5" s="4" t="n">
+        <f aca="false">STDEV(B5:K5)</f>
+        <v>0.231755018464182</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>0.9357</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>0.92395</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>0.45555</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>0.8083</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>0.89835</v>
+      </c>
+      <c r="G6" s="4" t="n">
+        <v>0.7863</v>
+      </c>
+      <c r="H6" s="4" t="n">
+        <v>0.98865</v>
+      </c>
+      <c r="I6" s="4" t="n">
+        <v>0.841</v>
+      </c>
+      <c r="J6" s="4" t="n">
+        <v>0.83665</v>
+      </c>
+      <c r="K6" s="4" t="n">
+        <v>0.8818</v>
+      </c>
+      <c r="M6" s="4" t="n">
+        <f aca="false">AVERAGE(B6:K6)</f>
+        <v>0.835625</v>
+      </c>
+      <c r="N6" s="4" t="n">
+        <f aca="false">STDEV(B6:K6)</f>
+        <v>0.147183210187545</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>0.90495</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>0.8155</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>0.94695</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>0.8283</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>0.78505</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>0.8373</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>0.89175</v>
+      </c>
+      <c r="I7" s="4" t="n">
+        <v>0.91505</v>
+      </c>
+      <c r="J7" s="4" t="n">
+        <v>0.73415</v>
+      </c>
+      <c r="K7" s="4" t="n">
+        <v>0.95535</v>
+      </c>
+      <c r="M7" s="4" t="n">
+        <f aca="false">AVERAGE(B7:K7)</f>
+        <v>0.861435</v>
+      </c>
+      <c r="N7" s="4" t="n">
+        <f aca="false">STDEV(B7:K7)</f>
+        <v>0.0727603030123188</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>0.8805</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>0.86865</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>0.9429</v>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>0.845</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>0.7254</v>
+      </c>
+      <c r="G8" s="4" t="n">
+        <v>0.8359</v>
+      </c>
+      <c r="H8" s="4" t="n">
+        <v>0.85965</v>
+      </c>
+      <c r="I8" s="4" t="n">
+        <v>0.93995</v>
+      </c>
+      <c r="J8" s="4" t="n">
+        <v>0.83095</v>
+      </c>
+      <c r="K8" s="4" t="n">
+        <v>0.9652</v>
+      </c>
+      <c r="M8" s="4" t="n">
+        <f aca="false">AVERAGE(B8:K8)</f>
+        <v>0.86941</v>
+      </c>
+      <c r="N8" s="4" t="n">
+        <f aca="false">STDEV(B8:K8)</f>
+        <v>0.0696882255318485</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="4" t="n">
+        <v>0.88195</v>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>0.7739</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>0.8224</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>0.8808</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <v>0.88325</v>
+      </c>
+      <c r="G9" s="4" t="n">
+        <v>0.83735</v>
+      </c>
+      <c r="H9" s="4" t="n">
+        <v>0.8964</v>
+      </c>
+      <c r="I9" s="4" t="n">
+        <v>0.92805</v>
+      </c>
+      <c r="J9" s="4" t="n">
+        <v>0.81625</v>
+      </c>
+      <c r="K9" s="4" t="n">
+        <v>0.8334</v>
+      </c>
+      <c r="M9" s="4" t="n">
+        <f aca="false">AVERAGE(B9:K9)</f>
+        <v>0.855375</v>
+      </c>
+      <c r="N9" s="4" t="n">
+        <f aca="false">STDEV(B9:K9)</f>
+        <v>0.0461380491929745</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="4" t="n">
+        <v>0.87925</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>0.75475</v>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>0.7836</v>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>0.84815</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>0.82355</v>
+      </c>
+      <c r="G10" s="4" t="n">
+        <v>0.92635</v>
+      </c>
+      <c r="H10" s="4" t="n">
+        <v>0.88115</v>
+      </c>
+      <c r="I10" s="4" t="n">
+        <v>0.9235</v>
+      </c>
+      <c r="J10" s="4" t="n">
+        <v>0.76525</v>
+      </c>
+      <c r="K10" s="4" t="n">
+        <v>0.77375</v>
+      </c>
+      <c r="M10" s="4" t="n">
+        <f aca="false">AVERAGE(B10:K10)</f>
+        <v>0.83593</v>
+      </c>
+      <c r="N10" s="4" t="n">
+        <f aca="false">STDEV(B10:K10)</f>
+        <v>0.0651996770612316</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="4" t="n">
+        <v>0.84845</v>
+      </c>
+      <c r="C11" s="4" t="n">
+        <v>0.4144</v>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>0.7575</v>
+      </c>
+      <c r="E11" s="4" t="n">
+        <v>0.8602</v>
+      </c>
+      <c r="F11" s="4" t="n">
+        <v>0.7858</v>
+      </c>
+      <c r="G11" s="4" t="n">
+        <v>0.666</v>
+      </c>
+      <c r="H11" s="4" t="n">
+        <v>0.72355</v>
+      </c>
+      <c r="I11" s="4" t="n">
+        <v>0.98665</v>
+      </c>
+      <c r="J11" s="4" t="n">
+        <v>0.8009</v>
+      </c>
+      <c r="K11" s="4" t="n">
+        <v>0.7064</v>
+      </c>
+      <c r="M11" s="4" t="n">
+        <f aca="false">AVERAGE(B11:K11)</f>
+        <v>0.754985</v>
+      </c>
+      <c r="N11" s="4" t="n">
+        <f aca="false">STDEV(B11:K11)</f>
+        <v>0.150482108663382</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="4" t="n">
+        <v>0.8124</v>
+      </c>
+      <c r="C12" s="4" t="n">
+        <v>0.44585</v>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>0.7662</v>
+      </c>
+      <c r="E12" s="4" t="n">
+        <v>0.81045</v>
+      </c>
+      <c r="F12" s="4" t="n">
+        <v>0.77985</v>
+      </c>
+      <c r="G12" s="4" t="n">
+        <v>0.62455</v>
+      </c>
+      <c r="H12" s="4" t="n">
+        <v>0.6313</v>
+      </c>
+      <c r="I12" s="4" t="n">
+        <v>0.47985</v>
+      </c>
+      <c r="J12" s="4" t="n">
+        <v>0.72575</v>
+      </c>
+      <c r="K12" s="4" t="n">
+        <v>0.7616</v>
+      </c>
+      <c r="M12" s="4" t="n">
+        <f aca="false">AVERAGE(B12:K12)</f>
+        <v>0.68378</v>
+      </c>
+      <c r="N12" s="4" t="n">
+        <f aca="false">STDEV(B12:K12)</f>
+        <v>0.133703154205293</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="4" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="C17" s="4" t="n">
+        <v>0.4219</v>
+      </c>
+      <c r="D17" s="4" t="n">
+        <v>0.81495</v>
+      </c>
+      <c r="E17" s="4" t="n">
+        <v>0.9018</v>
+      </c>
+      <c r="F17" s="4" t="n">
+        <v>0.8053</v>
+      </c>
+      <c r="G17" s="4" t="n">
+        <v>0.44185</v>
+      </c>
+      <c r="H17" s="4" t="n">
+        <v>0.8278</v>
+      </c>
+      <c r="I17" s="4" t="n">
+        <v>0.462</v>
+      </c>
+      <c r="J17" s="4" t="n">
+        <v>0.83975</v>
+      </c>
+      <c r="K17" s="4" t="n">
+        <v>0.7955</v>
+      </c>
+      <c r="M17" s="4" t="n">
+        <f aca="false">AVERAGE(B17:K17)</f>
+        <v>0.704085</v>
+      </c>
+      <c r="N17" s="4" t="n">
+        <f aca="false">STDEV(B17:K17)</f>
+        <v>0.186000640754571</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="4" t="n">
+        <v>0.59465</v>
+      </c>
+      <c r="C18" s="4" t="n">
+        <v>0.438</v>
+      </c>
+      <c r="D18" s="4" t="n">
+        <v>0.83215</v>
+      </c>
+      <c r="E18" s="4" t="n">
+        <v>0.79985</v>
+      </c>
+      <c r="F18" s="4" t="n">
+        <v>0.7785</v>
+      </c>
+      <c r="G18" s="4" t="n">
+        <v>0.60785</v>
+      </c>
+      <c r="H18" s="4" t="n">
+        <v>0.7315</v>
+      </c>
+      <c r="I18" s="4" t="n">
+        <v>0.7689</v>
+      </c>
+      <c r="J18" s="4" t="n">
+        <v>0.82495</v>
+      </c>
+      <c r="K18" s="4" t="n">
+        <v>0.82845</v>
+      </c>
+      <c r="M18" s="4" t="n">
+        <f aca="false">AVERAGE(B18:K18)</f>
+        <v>0.72048</v>
+      </c>
+      <c r="N18" s="4" t="n">
+        <f aca="false">STDEV(B18:K18)</f>
+        <v>0.131439551378825</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="4" t="n">
+        <v>0.8704</v>
+      </c>
+      <c r="C19" s="4" t="n">
+        <v>0.87675</v>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>0.3287</v>
+      </c>
+      <c r="E19" s="4" t="n">
+        <v>0.42645</v>
+      </c>
+      <c r="F19" s="4" t="n">
+        <v>0.3911</v>
+      </c>
+      <c r="G19" s="4" t="n">
+        <v>0.8502</v>
+      </c>
+      <c r="H19" s="4" t="n">
+        <v>0.70685</v>
+      </c>
+      <c r="I19" s="4" t="n">
+        <v>0.8729</v>
+      </c>
+      <c r="J19" s="4" t="n">
+        <v>0.87205</v>
+      </c>
+      <c r="K19" s="4" t="n">
+        <v>0.8702</v>
+      </c>
+      <c r="M19" s="4" t="n">
+        <f aca="false">AVERAGE(B19:K19)</f>
+        <v>0.70656</v>
+      </c>
+      <c r="N19" s="4" t="n">
+        <f aca="false">STDEV(B19:K19)</f>
+        <v>0.230706524494745</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="4" t="n">
+        <v>0.8309</v>
+      </c>
+      <c r="C20" s="4" t="n">
+        <v>0.7831</v>
+      </c>
+      <c r="D20" s="4" t="n">
+        <v>0.37275</v>
+      </c>
+      <c r="E20" s="4" t="n">
+        <v>0.8105</v>
+      </c>
+      <c r="F20" s="4" t="n">
+        <v>0.86225</v>
+      </c>
+      <c r="G20" s="4" t="n">
+        <v>0.85575</v>
+      </c>
+      <c r="H20" s="4" t="n">
+        <v>0.80205</v>
+      </c>
+      <c r="I20" s="4" t="n">
+        <v>0.8516</v>
+      </c>
+      <c r="J20" s="4" t="n">
+        <v>0.86525</v>
+      </c>
+      <c r="K20" s="4" t="n">
+        <v>0.8715</v>
+      </c>
+      <c r="M20" s="4" t="n">
+        <f aca="false">AVERAGE(B20:K20)</f>
+        <v>0.790565</v>
+      </c>
+      <c r="N20" s="4" t="n">
+        <f aca="false">STDEV(B20:K20)</f>
+        <v>0.149823132856341</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="4" t="n">
+        <v>0.85625</v>
+      </c>
+      <c r="C21" s="4" t="n">
+        <v>0.75635</v>
+      </c>
+      <c r="D21" s="4" t="n">
+        <v>0.8846</v>
+      </c>
+      <c r="E21" s="4" t="n">
+        <v>0.8731</v>
+      </c>
+      <c r="F21" s="4" t="n">
+        <v>0.8564</v>
+      </c>
+      <c r="G21" s="4" t="n">
+        <v>0.8798</v>
+      </c>
+      <c r="H21" s="4" t="n">
+        <v>0.87165</v>
+      </c>
+      <c r="I21" s="4" t="n">
+        <v>0.90825</v>
+      </c>
+      <c r="J21" s="4" t="n">
+        <v>0.80145</v>
+      </c>
+      <c r="K21" s="4" t="n">
+        <v>0.8348</v>
+      </c>
+      <c r="M21" s="4" t="n">
+        <f aca="false">AVERAGE(B21:K21)</f>
+        <v>0.852265</v>
+      </c>
+      <c r="N21" s="4" t="n">
+        <f aca="false">STDEV(B21:K21)</f>
+        <v>0.0445568055033871</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="4" t="n">
+        <v>0.8862</v>
+      </c>
+      <c r="C22" s="4" t="n">
+        <v>0.85045</v>
+      </c>
+      <c r="D22" s="4" t="n">
+        <v>0.86485</v>
+      </c>
+      <c r="E22" s="4" t="n">
+        <v>0.857</v>
+      </c>
+      <c r="F22" s="4" t="n">
+        <v>0.819</v>
+      </c>
+      <c r="G22" s="4" t="n">
+        <v>0.87055</v>
+      </c>
+      <c r="H22" s="4" t="n">
+        <v>0.87095</v>
+      </c>
+      <c r="I22" s="4" t="n">
+        <v>0.93045</v>
+      </c>
+      <c r="J22" s="4" t="n">
+        <v>0.8721</v>
+      </c>
+      <c r="K22" s="4" t="n">
+        <v>0.8201</v>
+      </c>
+      <c r="M22" s="4" t="n">
+        <f aca="false">AVERAGE(B22:K22)</f>
+        <v>0.864165</v>
+      </c>
+      <c r="N22" s="4" t="n">
+        <f aca="false">STDEV(B22:K22)</f>
+        <v>0.0320598749737633</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="4" t="n">
+        <v>0.79765</v>
+      </c>
+      <c r="C23" s="4" t="n">
+        <v>0.77015</v>
+      </c>
+      <c r="D23" s="4" t="n">
+        <v>0.84605</v>
+      </c>
+      <c r="E23" s="4" t="n">
+        <v>0.86755</v>
+      </c>
+      <c r="F23" s="4" t="n">
+        <v>0.86635</v>
+      </c>
+      <c r="G23" s="4" t="n">
+        <v>0.8574</v>
+      </c>
+      <c r="H23" s="4" t="n">
+        <v>0.83085</v>
+      </c>
+      <c r="I23" s="4" t="n">
+        <v>0.7596</v>
+      </c>
+      <c r="J23" s="4" t="n">
+        <v>0.85915</v>
+      </c>
+      <c r="K23" s="4" t="n">
+        <v>0.7517</v>
+      </c>
+      <c r="M23" s="4" t="n">
+        <f aca="false">AVERAGE(B23:K23)</f>
+        <v>0.820645</v>
+      </c>
+      <c r="N23" s="4" t="n">
+        <f aca="false">STDEV(B23:K23)</f>
+        <v>0.0464645232049858</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="4" t="n">
+        <v>0.85665</v>
+      </c>
+      <c r="C24" s="4" t="n">
+        <v>0.754</v>
+      </c>
+      <c r="D24" s="4" t="n">
+        <v>0.78595</v>
+      </c>
+      <c r="E24" s="4" t="n">
+        <v>0.8463</v>
+      </c>
+      <c r="F24" s="4" t="n">
+        <v>0.8484</v>
+      </c>
+      <c r="G24" s="4" t="n">
+        <v>0.81485</v>
+      </c>
+      <c r="H24" s="4" t="n">
+        <v>0.82275</v>
+      </c>
+      <c r="I24" s="4" t="n">
+        <v>0.77545</v>
+      </c>
+      <c r="J24" s="4" t="n">
+        <v>0.8235</v>
+      </c>
+      <c r="K24" s="4" t="n">
+        <v>0.8043</v>
+      </c>
+      <c r="M24" s="4" t="n">
+        <f aca="false">AVERAGE(B24:K24)</f>
+        <v>0.813215</v>
+      </c>
+      <c r="N24" s="4" t="n">
+        <f aca="false">STDEV(B24:K24)</f>
+        <v>0.0336221491976148</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="4" t="n">
+        <v>0.73555</v>
+      </c>
+      <c r="C25" s="4" t="n">
+        <v>0.40095</v>
+      </c>
+      <c r="D25" s="4" t="n">
+        <v>0.67985</v>
+      </c>
+      <c r="E25" s="4" t="n">
+        <v>0.73545</v>
+      </c>
+      <c r="F25" s="4" t="n">
+        <v>0.79435</v>
+      </c>
+      <c r="G25" s="4" t="n">
+        <v>0.6665</v>
+      </c>
+      <c r="H25" s="4" t="n">
+        <v>0.7529</v>
+      </c>
+      <c r="I25" s="4" t="n">
+        <v>0.29805</v>
+      </c>
+      <c r="J25" s="4" t="n">
+        <v>0.7739</v>
+      </c>
+      <c r="K25" s="4" t="n">
+        <v>0.7602</v>
+      </c>
+      <c r="M25" s="4" t="n">
+        <f aca="false">AVERAGE(B25:K25)</f>
+        <v>0.65977</v>
+      </c>
+      <c r="N25" s="4" t="n">
+        <f aca="false">STDEV(B25:K25)</f>
+        <v>0.169851090337651</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="4" t="n">
+        <v>0.745</v>
+      </c>
+      <c r="C26" s="4" t="n">
+        <v>0.426</v>
+      </c>
+      <c r="D26" s="4" t="n">
+        <v>0.6488</v>
+      </c>
+      <c r="E26" s="4" t="n">
+        <v>0.7234</v>
+      </c>
+      <c r="F26" s="4" t="n">
+        <v>0.78655</v>
+      </c>
+      <c r="G26" s="4" t="n">
+        <v>0.66605</v>
+      </c>
+      <c r="H26" s="4" t="n">
+        <v>0.5996</v>
+      </c>
+      <c r="I26" s="4" t="n">
+        <v>0.13755</v>
+      </c>
+      <c r="J26" s="4" t="n">
+        <v>0.6965</v>
+      </c>
+      <c r="K26" s="4" t="n">
+        <v>0.793</v>
+      </c>
+      <c r="M26" s="4" t="n">
+        <f aca="false">AVERAGE(B26:K26)</f>
+        <v>0.622245</v>
+      </c>
+      <c r="N26" s="4" t="n">
+        <f aca="false">STDEV(B26:K26)</f>
+        <v>0.20098272928842</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>